<commit_message>
Functioning x and y axis position control
</commit_message>
<xml_diff>
--- a/4_Paddle_Controller/Paddle_Controller_System_Sizing.xlsx
+++ b/4_Paddle_Controller/Paddle_Controller_System_Sizing.xlsx
@@ -2189,7 +2189,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2310,7 +2309,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2414,7 +2412,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2513,7 +2510,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4912,7 +4908,7 @@
   <dimension ref="A1:X332"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14939,7 +14935,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Improved robustness for position control
</commit_message>
<xml_diff>
--- a/4_Paddle_Controller/Paddle_Controller_System_Sizing.xlsx
+++ b/4_Paddle_Controller/Paddle_Controller_System_Sizing.xlsx
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>Pulley pitch diameter (m)</t>
-  </si>
-  <si>
-    <t>Load independed resistance (Nm)</t>
   </si>
   <si>
     <t>Coefficient of dynamic friction</t>
@@ -187,6 +184,9 @@
   </si>
   <si>
     <t>M5 Wing Nut</t>
+  </si>
+  <si>
+    <t>Load independet resistance (Nm)</t>
   </si>
 </sst>
 </file>
@@ -2189,6 +2189,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2309,6 +2310,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2412,6 +2414,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2510,6 +2513,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4907,8 +4911,8 @@
   </sheetPr>
   <dimension ref="A1:X332"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4932,18 +4936,18 @@
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="V3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="V4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
@@ -4958,22 +4962,22 @@
       <c r="E5" s="4"/>
       <c r="F5" s="5"/>
       <c r="I5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" t="s">
         <v>11</v>
       </c>
-      <c r="J5" t="s">
-        <v>12</v>
-      </c>
       <c r="K5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="V5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="W5">
         <v>3000</v>
       </c>
       <c r="X5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -5002,7 +5006,7 @@
         <v>0.32085561497326209</v>
       </c>
       <c r="X6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
@@ -5028,18 +5032,18 @@
         <v>13.333333333333334</v>
       </c>
       <c r="V7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="W7">
         <v>1.6</v>
       </c>
       <c r="X7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="12">
         <f>B7*10000</f>
@@ -5050,7 +5054,7 @@
       <c r="E8" s="12"/>
       <c r="F8" s="13"/>
       <c r="I8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J8">
         <f>($I$7-$I$6)/(J7-J6)</f>
@@ -5061,29 +5065,29 @@
         <v>-3.0890947499999998E-2</v>
       </c>
       <c r="V8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="W8">
         <v>0.48631578813043097</v>
       </c>
       <c r="X8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="V9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="W9">
         <v>8</v>
       </c>
       <c r="X9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="B10" s="19">
         <v>8</v>
@@ -5094,7 +5098,7 @@
       <c r="F10" s="5"/>
       <c r="I10" s="22"/>
       <c r="V10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="W10">
         <v>0.1</v>
@@ -5102,7 +5106,7 @@
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" s="17">
         <v>0.1</v>
@@ -5112,7 +5116,7 @@
       <c r="E11" s="8"/>
       <c r="F11" s="9"/>
       <c r="V11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="W11">
         <v>7.4999999999999997E-2</v>
@@ -5120,7 +5124,7 @@
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" s="7">
         <v>9.8000000000000007</v>
@@ -5132,7 +5136,7 @@
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" s="17">
         <v>1</v>
@@ -5144,7 +5148,7 @@
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" s="15">
         <f>(B11*B12*B13)+B10</f>
@@ -5157,7 +5161,7 @@
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16">
         <v>0.76454999999999995</v>
@@ -5165,21 +5169,21 @@
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
+        <v>28</v>
+      </c>
+      <c r="K19" t="s">
         <v>29</v>
       </c>
-      <c r="K19" t="s">
-        <v>30</v>
-      </c>
       <c r="U19" t="s">
+        <v>15</v>
+      </c>
+      <c r="X19" t="s">
         <v>16</v>
-      </c>
-      <c r="X19" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <f>B7</f>
@@ -5188,7 +5192,7 @@
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <f>B14</f>
@@ -5197,7 +5201,7 @@
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23">
         <f>-K8</f>
@@ -5206,7 +5210,7 @@
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" s="3">
         <f>I6</f>
@@ -5218,7 +5222,7 @@
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25">
         <f>B13</f>
@@ -5241,19 +5245,19 @@
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="T28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
@@ -5274,16 +5278,16 @@
         <v>0</v>
       </c>
       <c r="T29" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U29" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="U29" s="2" t="s">
+      <c r="V29" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="V29" s="2" t="s">
+      <c r="W29" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="W29" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
@@ -14946,12 +14950,12 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2">
         <v>90</v>
@@ -14959,7 +14963,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G3">
         <v>5</v>
@@ -14967,7 +14971,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G4">
         <v>5</v>
@@ -14975,12 +14979,12 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6">
         <v>50</v>
@@ -14988,7 +14992,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7">
         <v>15</v>
@@ -14996,7 +15000,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8">
         <v>195</v>
@@ -15004,7 +15008,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9">
         <v>75</v>
@@ -15012,7 +15016,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B11">
         <f>SUM(B2:B10)</f>

</xml_diff>

<commit_message>
Adding limit switch design and more PC design documents
</commit_message>
<xml_diff>
--- a/4_Paddle_Controller/Paddle_Controller_System_Sizing.xlsx
+++ b/4_Paddle_Controller/Paddle_Controller_System_Sizing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Calculations" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="67">
   <si>
     <t>Paddle Controller System Sizing</t>
   </si>
@@ -188,11 +188,56 @@
   <si>
     <t>Load independet resistance (Nm)</t>
   </si>
+  <si>
+    <t>Rod Volume</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>OD</t>
+  </si>
+  <si>
+    <t>Thickness</t>
+  </si>
+  <si>
+    <t>OA</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>Net Area</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>in^3</t>
+  </si>
+  <si>
+    <t>Density</t>
+  </si>
+  <si>
+    <t>lb/in^3</t>
+  </si>
+  <si>
+    <t>lb</t>
+  </si>
+  <si>
+    <t>grams</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -348,7 +393,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2189,7 +2234,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2310,7 +2354,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2414,7 +2457,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2513,7 +2555,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4911,8 +4952,8 @@
   </sheetPr>
   <dimension ref="A1:X332"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14936,10 +14977,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14948,12 +14989,12 @@
     <col min="6" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -14961,7 +15002,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F3" t="s">
         <v>50</v>
       </c>
@@ -14969,7 +15010,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
         <v>51</v>
       </c>
@@ -14977,50 +15018,147 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>49</v>
       </c>
       <c r="B6">
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="O6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>48</v>
       </c>
       <c r="B7">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="O7" t="s">
+        <v>55</v>
+      </c>
+      <c r="P7">
+        <v>0.5</v>
+      </c>
+      <c r="R7" t="s">
+        <v>57</v>
+      </c>
+      <c r="S7">
+        <f>PI()*(P7/2)^2</f>
+        <v>0.19634954084936207</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>45</v>
       </c>
       <c r="B8">
         <v>195</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="O8" t="s">
+        <v>56</v>
+      </c>
+      <c r="P8">
+        <v>6.5000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>46</v>
       </c>
       <c r="B9">
         <v>75</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="O9" t="s">
+        <v>54</v>
+      </c>
+      <c r="P9">
+        <f>P7-P8</f>
+        <v>0.435</v>
+      </c>
+      <c r="R9" t="s">
+        <v>58</v>
+      </c>
+      <c r="S9">
+        <f t="shared" ref="S8:S9" si="0">PI()*(P9/2)^2</f>
+        <v>0.14861696746888214</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R10" t="s">
+        <v>59</v>
+      </c>
+      <c r="S10">
+        <f>S7-S9</f>
+        <v>4.7732573380479926E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>47</v>
       </c>
       <c r="B11">
         <f>SUM(B2:B10)</f>
         <v>425</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R12" t="s">
+        <v>60</v>
+      </c>
+      <c r="S12">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R13" t="s">
+        <v>61</v>
+      </c>
+      <c r="S13">
+        <f>S10*S12</f>
+        <v>1.8138377884582373</v>
+      </c>
+      <c r="T13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R15" t="s">
+        <v>63</v>
+      </c>
+      <c r="S15">
+        <v>9.7500000000000003E-2</v>
+      </c>
+      <c r="T15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R16" t="s">
+        <v>41</v>
+      </c>
+      <c r="S16">
+        <f>S13*S15</f>
+        <v>0.17684918437467814</v>
+      </c>
+      <c r="T16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="19:20" x14ac:dyDescent="0.25">
+      <c r="S17">
+        <f>S16*453.592</f>
+        <v>80.217375238879001</v>
+      </c>
+      <c r="T17" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>